<commit_message>
Processing and dynamic mapping logic implemented
</commit_message>
<xml_diff>
--- a/DataFiles/ProcessingWorkbook.xlsx
+++ b/DataFiles/ProcessingWorkbook.xlsx
@@ -8,7 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="StudentPreferences" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="StudentsMapping" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="OrganizationMapping" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -979,6 +981,648 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>USC ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Student Name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>6:00 - 6:07pm</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>6:10 - 6:17pm</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>6:20 - 6:27pm</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>6:30 - 6:37pm</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>10001</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Oceana Hanner</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Cedars-Sinai - Neurosciences</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Keck VIO - COBI</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Optum CF - Patient XP</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Providence Health Network</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>10002</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Esther Choi</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Keck VIO - COBI</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Optum CF - Patient XP</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">St.Johns-PhysPartners </t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Verdugo Hills Hospital</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>10003</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Daniela Ahumada</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>City of Hope - CMO</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>CHLA - Anesthesia&amp;CCM</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Providence Health Network</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Optum CF - Patient XP</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>10004</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Fahima Gohil</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Rancho Los Amigos NRC</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Cedars-Sinai - Neurosciences</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Emanate Health</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>City of Hope - CMO</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>10005</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Julia Orozco</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Emanate Health</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Providence Health Network</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Keck VIO - COBI</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Kaiser PC - Consulting</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>10006</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Emma Crusinberry</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Kaiser PC - Consulting</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">St.Johns-PhysPartners </t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>SCAN Health Plan</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Cedars-Sinai - Neurosciences</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>10007</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Stanley Ibe</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Optum CF - Patient XP</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>City of Hope - CMO</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>CHLA - Anesthesia&amp;CCM</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">St.Johns-PhysPartners </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>10008</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Raashi Subramanya</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Providence Health Network</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>SCAN Health Plan</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Cedars-Sinai - Neurosciences</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Keck VIO - COBI</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Organization Code</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Organization Name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>6:00 - 6:07pm</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>6:10 - 6:17pm</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>6:20 - 6:27pm</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>6:30 - 6:37pm</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>C0</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Cedars-Sinai - Neurosciences</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>10001</v>
+      </c>
+      <c r="D2" t="n">
+        <v>10004</v>
+      </c>
+      <c r="E2" t="n">
+        <v>10008</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10006</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>CHLA - Anesthesia&amp;CCM</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>10003</v>
+      </c>
+      <c r="E3" t="n">
+        <v>10007</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>City of Hope - CMO</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>10003</v>
+      </c>
+      <c r="D4" t="n">
+        <v>10007</v>
+      </c>
+      <c r="F4" t="n">
+        <v>10004</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>E0</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Emanate Health</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>10005</v>
+      </c>
+      <c r="E5" t="n">
+        <v>10004</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>K0</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Kaiser PC - Consulting</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>10006</v>
+      </c>
+      <c r="F6" t="n">
+        <v>10005</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>K1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Keck IRM</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>K2</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Keck VIO - COBI</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>10002</v>
+      </c>
+      <c r="D8" t="n">
+        <v>10001</v>
+      </c>
+      <c r="E8" t="n">
+        <v>10005</v>
+      </c>
+      <c r="F8" t="n">
+        <v>10008</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>O0</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Optum CF - Digi Transformation</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>O1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Optum CF - Patient XP</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>10007</v>
+      </c>
+      <c r="D10" t="n">
+        <v>10002</v>
+      </c>
+      <c r="E10" t="n">
+        <v>10001</v>
+      </c>
+      <c r="F10" t="n">
+        <v>10003</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>P0</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Providence Health Network</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Providence Health Network</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>10008</v>
+      </c>
+      <c r="D12" t="n">
+        <v>10005</v>
+      </c>
+      <c r="E12" t="n">
+        <v>10003</v>
+      </c>
+      <c r="F12" t="n">
+        <v>10001</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>R0</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Rancho Los Amigos NRC</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>10004</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>S0</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SCAN Health Plan</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>10008</v>
+      </c>
+      <c r="E14" t="n">
+        <v>10006</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">St.Johns-PhysPartners </t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>10006</v>
+      </c>
+      <c r="E15" t="n">
+        <v>10002</v>
+      </c>
+      <c r="F15" t="n">
+        <v>10007</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>T0</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Torrance Memorial</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>V0</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Verdugo Hills Hospital</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>10002</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>W0</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>West Hills Hospital</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Change in TimeSheet input sheet format
</commit_message>
<xml_diff>
--- a/DataFiles/ProcessingWorkbook.xlsx
+++ b/DataFiles/ProcessingWorkbook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="StudentPreferences"/>
@@ -296,16 +296,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B1:B17" displayName="Table1" name="Table1" id="1" totalsRowShown="0">
-  <autoFilter ref="B1:B17"/>
-  <tableColumns count="1">
-    <tableColumn name="Organization Name" id="1" totalsRowLabel="Total"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1122,16 +1112,16 @@
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="21.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="29.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="34.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="33.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="33.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -1406,16 +1396,16 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="30.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="23.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="20.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="21.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -1728,9 +1718,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>